<commit_message>
added user trial data
</commit_message>
<xml_diff>
--- a/user-data.xlsx
+++ b/user-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9810" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Subject 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="12">
   <si>
     <t>10uL</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>15% error Max</t>
+  </si>
+  <si>
+    <t>0.0.0094</t>
   </si>
 </sst>
 </file>
@@ -385,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,57 +420,93 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>0.18540000000000001</v>
+      </c>
+      <c r="C3">
+        <v>4.1300000000000003E-2</v>
+      </c>
+      <c r="D3">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="E3">
+        <v>9.4000000000000004E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.18529999999999999</v>
+      </c>
+      <c r="C4">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="E4">
+        <v>9.4000000000000004E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>0.18529999999999999</v>
+      </c>
+      <c r="C5">
+        <v>3.9100000000000003E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="E5">
+        <v>9.1999999999999998E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="e">
+      <c r="B6">
         <f>AVERAGE(B3:B5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" t="e">
+        <v>0.18533333333333335</v>
+      </c>
+      <c r="C6">
         <f>AVERAGE(C3:C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" t="e">
+        <v>3.9866666666666668E-2</v>
+      </c>
+      <c r="D6">
         <f>AVERAGE(D3:D5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" t="e">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="E6">
         <f>AVERAGE(E3:E5)</f>
-        <v>#DIV/0!</v>
+        <v>9.3333333333333341E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="e">
+      <c r="B7">
         <f>(0.2-B6)*100/0.2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" t="e">
+        <v>7.3333333333333304</v>
+      </c>
+      <c r="C7">
         <f>(0.05-C6)*100/0.05</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" t="e">
+        <v>20.266666666666666</v>
+      </c>
+      <c r="D7">
         <f>(0.02-D6)*100/0.02</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" t="e">
+        <v>13.000000000000009</v>
+      </c>
+      <c r="E7">
         <f>(0.01-E6)*100/0.01</f>
-        <v>#DIV/0!</v>
+        <v>6.6666666666666607</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -492,6 +531,18 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="C13">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D13">
+        <v>2.07E-2</v>
+      </c>
+      <c r="E13">
+        <v>9.4000000000000004E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -843,7 +894,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,57 +922,93 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>0.1822</v>
+      </c>
+      <c r="C3">
+        <v>4.1099999999999998E-2</v>
+      </c>
+      <c r="D3">
+        <v>1.83E-2</v>
+      </c>
+      <c r="E3">
+        <v>8.6999999999999994E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.17860000000000001</v>
+      </c>
+      <c r="C4">
+        <v>4.1399999999999999E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="E4">
+        <v>8.6999999999999994E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>0.1782</v>
+      </c>
+      <c r="C5">
+        <v>4.0899999999999999E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.84E-2</v>
+      </c>
+      <c r="E5">
+        <v>7.7000000000000002E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="e">
+      <c r="B6">
         <f>AVERAGE(B3:B5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" t="e">
+        <v>0.17966666666666667</v>
+      </c>
+      <c r="C6">
         <f>AVERAGE(C3:C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" t="e">
+        <v>4.1133333333333327E-2</v>
+      </c>
+      <c r="D6">
         <f>AVERAGE(D3:D5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" t="e">
+        <v>1.8466666666666669E-2</v>
+      </c>
+      <c r="E6">
         <f>AVERAGE(E3:E5)</f>
-        <v>#DIV/0!</v>
+        <v>8.3666666666666663E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="e">
+      <c r="B7">
         <f>(0.2-B6)*100/0.2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" t="e">
+        <v>10.16666666666667</v>
+      </c>
+      <c r="C7">
         <f>(0.05-C6)*100/0.05</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" t="e">
+        <v>17.733333333333352</v>
+      </c>
+      <c r="D7">
         <f>(0.02-D6)*100/0.02</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" t="e">
+        <v>7.6666666666666545</v>
+      </c>
+      <c r="E7">
         <f>(0.01-E6)*100/0.01</f>
-        <v>#DIV/0!</v>
+        <v>16.333333333333339</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -946,6 +1033,18 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="C13">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="D13">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="E13">
+        <v>1.11E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,7 +1169,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,57 +1197,93 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>0.27610000000000001</v>
+      </c>
+      <c r="C3">
+        <v>4.4499999999999998E-2</v>
+      </c>
+      <c r="D3">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="E3">
+        <v>1.6999999999999999E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.27910000000000001</v>
+      </c>
+      <c r="C4">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="D4">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="E4">
+        <v>7.4000000000000003E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>0.27429999999999999</v>
+      </c>
+      <c r="C5">
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="D5">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E5">
+        <v>7.7999999999999996E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="e">
+      <c r="B6">
         <f>AVERAGE(B3:B5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" t="e">
+        <v>0.27650000000000002</v>
+      </c>
+      <c r="C6">
         <f>AVERAGE(C3:C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" t="e">
+        <v>4.4199999999999996E-2</v>
+      </c>
+      <c r="D6">
         <f>AVERAGE(D3:D5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" t="e">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="E6">
         <f>AVERAGE(E3:E5)</f>
-        <v>#DIV/0!</v>
+        <v>5.6333333333333331E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="e">
-        <f>(0.2-B6)*100/0.2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" t="e">
+      <c r="B7">
+        <f>(B6-0.2)*100/0.2</f>
+        <v>38.250000000000007</v>
+      </c>
+      <c r="C7">
         <f>(0.05-C6)*100/0.05</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" t="e">
+        <v>11.600000000000012</v>
+      </c>
+      <c r="D7">
         <f>(0.02-D6)*100/0.02</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" t="e">
+        <v>69</v>
+      </c>
+      <c r="E7">
         <f>(0.01-E6)*100/0.01</f>
-        <v>#DIV/0!</v>
+        <v>43.666666666666671</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1174,25 +1309,49 @@
       <c r="A13">
         <v>1</v>
       </c>
+      <c r="B13">
+        <v>0.18390000000000001</v>
+      </c>
+      <c r="C13">
+        <v>4.7800000000000004E-3</v>
+      </c>
+      <c r="D13">
+        <v>1.11E-2</v>
+      </c>
+      <c r="E13">
+        <v>1.09E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
+      </c>
+      <c r="D14">
+        <v>1.34E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
+      <c r="D15">
+        <v>3.1099999999999999E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
+      <c r="D16">
+        <v>1.67E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
+      </c>
+      <c r="D17">
+        <v>1.8700000000000001E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1297,7 +1456,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,57 +1484,93 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>0.1847</v>
+      </c>
+      <c r="C3">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="D3">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="E3">
+        <v>1.15E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.18429999999999999</v>
+      </c>
+      <c r="C4">
+        <v>4.0300000000000002E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="E4">
+        <v>1.15E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>0.1845</v>
+      </c>
+      <c r="C5">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1.17E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="e">
+      <c r="B6">
         <f>AVERAGE(B3:B5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" t="e">
+        <v>0.1845</v>
+      </c>
+      <c r="C6">
         <f>AVERAGE(C3:C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" t="e">
+        <v>4.003333333333333E-2</v>
+      </c>
+      <c r="D6">
         <f>AVERAGE(D3:D5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" t="e">
+        <v>1.2299999999999998E-2</v>
+      </c>
+      <c r="E6">
         <f>AVERAGE(E3:E5)</f>
-        <v>#DIV/0!</v>
+        <v>1.1566666666666668E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="e">
+      <c r="B7">
         <f>(0.2-B6)*100/0.2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" t="e">
+        <v>7.7500000000000062</v>
+      </c>
+      <c r="C7">
         <f>(0.05-C6)*100/0.05</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" t="e">
+        <v>19.933333333333344</v>
+      </c>
+      <c r="D7">
         <f>(0.02-D6)*100/0.02</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" t="e">
-        <f>(0.01-E6)*100/0.01</f>
-        <v>#DIV/0!</v>
+        <v>38.500000000000014</v>
+      </c>
+      <c r="E7">
+        <f>(E6-0.01)*100/0.01</f>
+        <v>15.666666666666675</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1400,6 +1595,18 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0.19209999999999999</v>
+      </c>
+      <c r="C13">
+        <v>4.8800000000000003E-2</v>
+      </c>
+      <c r="D13">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="E13">
+        <v>9.4000000000000004E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1524,7 +1731,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,57 +1759,93 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>0.1915</v>
+      </c>
+      <c r="C3">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="D3">
+        <v>2.01E-2</v>
+      </c>
+      <c r="E3">
+        <v>3.8E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.1913</v>
+      </c>
+      <c r="C4">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.02</v>
+      </c>
+      <c r="E4">
+        <v>2.0999999999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>0.1913</v>
+      </c>
+      <c r="C5">
+        <v>5.16E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="E5">
+        <v>1.6000000000000001E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="e">
+      <c r="B6">
         <f>AVERAGE(B3:B5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" t="e">
+        <v>0.19136666666666668</v>
+      </c>
+      <c r="C6">
         <f>AVERAGE(C3:C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" t="e">
+        <v>5.0300000000000004E-2</v>
+      </c>
+      <c r="D6">
         <f>AVERAGE(D3:D5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" t="e">
+        <v>1.9966666666666664E-2</v>
+      </c>
+      <c r="E6">
         <f>AVERAGE(E3:E5)</f>
-        <v>#DIV/0!</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="e">
+      <c r="B7">
         <f>(0.2-B6)*100/0.2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" t="e">
+        <v>4.3166666666666629</v>
+      </c>
+      <c r="C7">
         <f>(0.05-C6)*100/0.05</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" t="e">
+        <v>-0.60000000000000331</v>
+      </c>
+      <c r="D7">
         <f>(0.02-D6)*100/0.02</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" t="e">
+        <v>0.16666666666668301</v>
+      </c>
+      <c r="E7">
         <f>(0.01-E6)*100/0.01</f>
-        <v>#DIV/0!</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1628,10 +1871,25 @@
       <c r="A13">
         <v>1</v>
       </c>
+      <c r="B13">
+        <v>0.19220000000000001</v>
+      </c>
+      <c r="C13">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="D13">
+        <v>2.01E-2</v>
+      </c>
+      <c r="E13">
+        <v>5.4999999999999997E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
+      </c>
+      <c r="E14">
+        <v>1.06E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1750,8 +2008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,57 +2037,93 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>0.192</v>
+      </c>
+      <c r="C3">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D3">
+        <v>1.78E-2</v>
+      </c>
+      <c r="E3">
+        <v>8.3000000000000001E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.193</v>
+      </c>
+      <c r="C4">
+        <v>4.58E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="E4">
+        <v>8.0999999999999996E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>0.19259999999999999</v>
+      </c>
+      <c r="C5">
+        <v>4.58E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>8.0999999999999996E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="e">
+      <c r="B6">
         <f>AVERAGE(B3:B5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" t="e">
+        <v>0.19253333333333333</v>
+      </c>
+      <c r="C6">
         <f>AVERAGE(C3:C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" t="e">
+        <v>4.6199999999999998E-2</v>
+      </c>
+      <c r="D6">
         <f>AVERAGE(D3:D5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" t="e">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="E6">
         <f>AVERAGE(E3:E5)</f>
-        <v>#DIV/0!</v>
+        <v>8.1666666666666658E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="e">
+      <c r="B7">
         <f>(0.2-B6)*100/0.2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" t="e">
+        <v>3.7333333333333383</v>
+      </c>
+      <c r="C7">
         <f>(0.05-C6)*100/0.05</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" t="e">
+        <v>7.6000000000000085</v>
+      </c>
+      <c r="D7">
         <f>(0.02-D6)*100/0.02</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" t="e">
+        <v>13.500000000000005</v>
+      </c>
+      <c r="E7">
         <f>(0.01-E6)*100/0.01</f>
-        <v>#DIV/0!</v>
+        <v>18.333333333333343</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1854,6 +2148,18 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0.193</v>
+      </c>
+      <c r="C13">
+        <v>4.6609999999999999E-2</v>
+      </c>
+      <c r="D13">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="E13">
+        <v>9.4999999999999998E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added suggestion from improving the trial
</commit_message>
<xml_diff>
--- a/user-data.xlsx
+++ b/user-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9810" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9810"/>
   </bookViews>
   <sheets>
     <sheet name="Subject 1" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -1730,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,8 +1836,8 @@
         <v>4.3166666666666629</v>
       </c>
       <c r="C7">
-        <f>(0.05-C6)*100/0.05</f>
-        <v>-0.60000000000000331</v>
+        <f>(0.05-C6)*100/-0.05</f>
+        <v>0.60000000000000331</v>
       </c>
       <c r="D7">
         <f>(0.02-D6)*100/0.02</f>
@@ -2008,7 +2008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>